<commit_message>
updating sulfur database files
</commit_message>
<xml_diff>
--- a/ocean_microbiomics_results/KOsToAdd.xlsx
+++ b/ocean_microbiomics_results/KOsToAdd.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Documents/DOSTraits/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Documents/GitHub/sulfurtraits/ocean_microbiomics_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0634393-C190-644B-A0DE-B1CC7C27B9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE77E4D-7E45-344A-8A9A-48B260F877BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{190E7DE5-6A20-5D48-966C-F9F0D2C31C62}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" activeTab="1" xr2:uid="{190E7DE5-6A20-5D48-966C-F9F0D2C31C62}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="pass1" sheetId="1" r:id="rId1"/>
+    <sheet name="pass2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>K00958</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>K15762</t>
+  </si>
+  <si>
+    <t>K01133</t>
+  </si>
+  <si>
+    <t>K05846</t>
+  </si>
+  <si>
+    <t>K05847</t>
   </si>
 </sst>
 </file>
@@ -497,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161DB376-FC67-C643-8007-05E014F7B921}">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -641,4 +650,34 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554463BF-62D6-8548-8DD9-DA5390E53A42}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update sulfur database and new KOs
</commit_message>
<xml_diff>
--- a/ocean_microbiomics_results/KOsToAdd.xlsx
+++ b/ocean_microbiomics_results/KOsToAdd.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Documents/GitHub/sulfurtraits/ocean_microbiomics_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE77E4D-7E45-344A-8A9A-48B260F877BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB9E942E-F03A-3D4B-A4B3-EF1148A5D7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" activeTab="1" xr2:uid="{190E7DE5-6A20-5D48-966C-F9F0D2C31C62}"/>
+    <workbookView xWindow="1000" yWindow="760" windowWidth="27640" windowHeight="16440" activeTab="1" xr2:uid="{190E7DE5-6A20-5D48-966C-F9F0D2C31C62}"/>
   </bookViews>
   <sheets>
     <sheet name="pass1" sheetId="1" r:id="rId1"/>
-    <sheet name="pass2" sheetId="2" r:id="rId2"/>
+    <sheet name="KOsToAdd" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>K00958</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>K05847</t>
+  </si>
+  <si>
+    <t>K00003</t>
+  </si>
+  <si>
+    <t>K27857</t>
+  </si>
+  <si>
+    <t>K00485</t>
+  </si>
+  <si>
+    <t>K20036</t>
   </si>
 </sst>
 </file>
@@ -654,10 +666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554463BF-62D6-8548-8DD9-DA5390E53A42}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,6 +689,29 @@
         <v>29</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>